<commit_message>
Map coordinates in Excel file
</commit_message>
<xml_diff>
--- a/data/37-intersection map EV1 Solution.xlsx
+++ b/data/37-intersection map EV1 Solution.xlsx
@@ -489,16 +489,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>16.17546152373445</v>
+        <v>16.1754615237336</v>
       </c>
       <c r="D2" t="n">
-        <v>16.17546152373445</v>
+        <v>16.1754615237336</v>
       </c>
       <c r="E2" t="n">
-        <v>9.364289244444707</v>
+        <v>9.364289244444443</v>
       </c>
       <c r="F2" t="n">
-        <v>9.364289244444707</v>
+        <v>9.364289244444443</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -512,16 +512,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>14.53785325040134</v>
+        <v>14.53785325040029</v>
       </c>
       <c r="D3" t="n">
-        <v>14.53785325040134</v>
+        <v>14.53785325040029</v>
       </c>
       <c r="E3" t="n">
-        <v>9.732904800000457</v>
+        <v>9.732904799999998</v>
       </c>
       <c r="F3" t="n">
-        <v>9.982904800000457</v>
+        <v>9.982904799999998</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -629,16 +629,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>14.35195164373484</v>
+        <v>14.35195164373362</v>
       </c>
       <c r="D8" t="n">
-        <v>14.35195164373484</v>
+        <v>14.35195164373362</v>
       </c>
       <c r="E8" t="n">
-        <v>10.02485368888939</v>
+        <v>10.02485368888889</v>
       </c>
       <c r="F8" t="n">
-        <v>10.02485368888939</v>
+        <v>10.02485368888889</v>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
@@ -652,16 +652,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>12.93654337040196</v>
+        <v>12.93654337040032</v>
       </c>
       <c r="D9" t="n">
-        <v>12.93654337040196</v>
+        <v>12.93654337040032</v>
       </c>
       <c r="E9" t="n">
-        <v>10.34346924444499</v>
+        <v>10.34346924444444</v>
       </c>
       <c r="F9" t="n">
-        <v>10.34346924444499</v>
+        <v>10.34346924444444</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
@@ -675,16 +675,16 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>10.70640176373543</v>
+        <v>10.70640176373369</v>
       </c>
       <c r="D10" t="n">
-        <v>10.70640176373543</v>
+        <v>10.70640176373369</v>
       </c>
       <c r="E10" t="n">
-        <v>10.84541813333392</v>
+        <v>10.84541813333333</v>
       </c>
       <c r="F10" t="n">
-        <v>11.09541813333392</v>
+        <v>11.09541813333333</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
@@ -700,16 +700,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>17.65894754853424</v>
+        <v>17.6589475485336</v>
       </c>
       <c r="D11" t="n">
-        <v>17.65894754853424</v>
+        <v>17.6589475485336</v>
       </c>
       <c r="E11" t="n">
-        <v>9.161042400000136</v>
+        <v>9.161042399999998</v>
       </c>
       <c r="F11" t="n">
-        <v>9.161042400000136</v>
+        <v>9.161042399999998</v>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
@@ -723,16 +723,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>18.41223357333408</v>
+        <v>18.41223357333357</v>
       </c>
       <c r="D12" t="n">
-        <v>18.41223357333413</v>
+        <v>18.41223357333357</v>
       </c>
       <c r="E12" t="n">
-        <v>9.05779555555565</v>
+        <v>9.057795555555554</v>
       </c>
       <c r="F12" t="n">
-        <v>9.057795555555659</v>
+        <v>9.057795555555554</v>
       </c>
       <c r="G12" t="n">
         <v>-0</v>
@@ -823,22 +823,22 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>10.17979349040221</v>
+        <v>10.17979349040035</v>
       </c>
       <c r="D16" t="n">
-        <v>22.89694160666666</v>
+        <v>22.8969416066667</v>
       </c>
       <c r="E16" t="n">
-        <v>11.21403368888949</v>
+        <v>11.21403368888889</v>
       </c>
       <c r="F16" t="n">
-        <v>14.8937640466049</v>
+        <v>14.89376404660485</v>
       </c>
       <c r="G16" t="n">
         <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>3.679730357715407</v>
+        <v>3.679730357715957</v>
       </c>
       <c r="I16" t="inlineStr"/>
     </row>
@@ -856,10 +856,10 @@
         <v>22</v>
       </c>
       <c r="E17" t="n">
-        <v>15.09571293549379</v>
+        <v>15.09571293549373</v>
       </c>
       <c r="F17" t="n">
-        <v>15.09571293549379</v>
+        <v>15.09571293549373</v>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
@@ -873,16 +873,16 @@
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>21.47339172666673</v>
+        <v>21.47339172666676</v>
       </c>
       <c r="D18" t="n">
-        <v>21.47339172666673</v>
+        <v>21.47339172666676</v>
       </c>
       <c r="E18" t="n">
-        <v>15.21432849104935</v>
+        <v>15.21432849104929</v>
       </c>
       <c r="F18" t="n">
-        <v>15.21432849104935</v>
+        <v>15.21432849104929</v>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
@@ -893,7 +893,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -919,16 +919,16 @@
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>19.38324184666727</v>
+        <v>19.3832418466669</v>
       </c>
       <c r="D20" t="n">
-        <v>19.38324184666727</v>
+        <v>19.3832418466669</v>
       </c>
       <c r="E20" t="n">
-        <v>8.589180000000036</v>
+        <v>8.589179999999999</v>
       </c>
       <c r="F20" t="n">
-        <v>8.839180000000036</v>
+        <v>8.839179999999999</v>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -941,7 +941,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -967,16 +967,16 @@
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>20.28018345333353</v>
+        <v>20.28018345333334</v>
       </c>
       <c r="D22" t="n">
-        <v>20.28018345333353</v>
+        <v>20.28018345333334</v>
       </c>
       <c r="E22" t="n">
-        <v>8.387231111111157</v>
+        <v>8.387231111111111</v>
       </c>
       <c r="F22" t="n">
-        <v>8.387231111111157</v>
+        <v>8.387231111111111</v>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
@@ -987,7 +987,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -1019,10 +1019,10 @@
         <v>20.95492506000001</v>
       </c>
       <c r="E24" t="n">
-        <v>8.23528222222223</v>
+        <v>8.235282222222223</v>
       </c>
       <c r="F24" t="n">
-        <v>8.23528222222223</v>
+        <v>8.235282222222223</v>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
@@ -1059,16 +1059,16 @@
         <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>16.19645421520013</v>
+        <v>16.1964542152001</v>
       </c>
       <c r="D26" t="n">
-        <v>16.19645421520013</v>
+        <v>16.1964542152001</v>
       </c>
       <c r="E26" t="n">
-        <v>16.47008866882712</v>
+        <v>16.47008866882707</v>
       </c>
       <c r="F26" t="n">
-        <v>16.72008866882712</v>
+        <v>16.72008866882707</v>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
@@ -1084,22 +1084,22 @@
         <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>14.71296819040013</v>
+        <v>14.71296819040009</v>
       </c>
       <c r="D27" t="n">
         <v>23.63760827333332</v>
       </c>
       <c r="E27" t="n">
-        <v>16.92333551327157</v>
+        <v>16.92333551327151</v>
       </c>
       <c r="F27" t="n">
-        <v>18.33189613242138</v>
+        <v>18.33189613242133</v>
       </c>
       <c r="G27" t="n">
         <v>1</v>
       </c>
       <c r="H27" t="n">
-        <v>1.408560619149809</v>
+        <v>1.408560619149816</v>
       </c>
       <c r="I27" t="inlineStr"/>
     </row>
@@ -1111,16 +1111,16 @@
         <v>1</v>
       </c>
       <c r="C28" t="n">
-        <v>18.2641002400001</v>
+        <v>18.26410024000009</v>
       </c>
       <c r="D28" t="n">
-        <v>18.2641002400001</v>
+        <v>18.26410024000009</v>
       </c>
       <c r="E28" t="n">
-        <v>16.18684182438268</v>
+        <v>16.18684182438262</v>
       </c>
       <c r="F28" t="n">
-        <v>16.18684182438268</v>
+        <v>16.18684182438262</v>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
@@ -1131,7 +1131,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -1157,16 +1157,16 @@
         <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>19.67950851333339</v>
+        <v>19.67950851333343</v>
       </c>
       <c r="D30" t="n">
-        <v>19.67950851333339</v>
+        <v>19.67950851333343</v>
       </c>
       <c r="E30" t="n">
-        <v>15.86822626882712</v>
+        <v>15.86822626882707</v>
       </c>
       <c r="F30" t="n">
-        <v>15.86822626882712</v>
+        <v>15.86822626882707</v>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
@@ -1180,16 +1180,16 @@
         <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>20.20611678666673</v>
+        <v>20.20611678666676</v>
       </c>
       <c r="D31" t="n">
-        <v>20.20611678666673</v>
+        <v>20.20611678666676</v>
       </c>
       <c r="E31" t="n">
-        <v>15.49961071327157</v>
+        <v>15.49961071327151</v>
       </c>
       <c r="F31" t="n">
-        <v>15.74961071327157</v>
+        <v>15.74961071327151</v>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
@@ -1202,7 +1202,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -1248,7 +1248,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -1317,7 +1317,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -1340,7 +1340,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -1355,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -1376,10 +1376,10 @@
         <v>22</v>
       </c>
       <c r="E39" t="n">
-        <v>18.70051168797694</v>
+        <v>18.70051168797688</v>
       </c>
       <c r="F39" t="n">
-        <v>18.70051168797694</v>
+        <v>18.70051168797688</v>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
@@ -1712,7 +1712,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
@@ -1725,7 +1725,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
@@ -1894,7 +1894,7 @@
         <v>31</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
@@ -1907,7 +1907,7 @@
         <v>27</v>
       </c>
       <c r="C38" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
@@ -1933,7 +1933,7 @@
         <v>29</v>
       </c>
       <c r="C40" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
@@ -1998,7 +1998,7 @@
         <v>28</v>
       </c>
       <c r="C45" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
@@ -2050,7 +2050,7 @@
         <v>20</v>
       </c>
       <c r="C49" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
@@ -2063,7 +2063,7 @@
         <v>22</v>
       </c>
       <c r="C50" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
@@ -2115,7 +2115,7 @@
         <v>27</v>
       </c>
       <c r="C54" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
@@ -2141,7 +2141,7 @@
         <v>37</v>
       </c>
       <c r="C56" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
@@ -2232,7 +2232,7 @@
         <v>30</v>
       </c>
       <c r="C63" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
@@ -2284,7 +2284,7 @@
         <v>36</v>
       </c>
       <c r="C67" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
@@ -2401,7 +2401,7 @@
         <v>37</v>
       </c>
       <c r="C76" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr"/>
@@ -2505,7 +2505,7 @@
         <v>1</v>
       </c>
       <c r="C84" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
@@ -2986,7 +2986,7 @@
         <v>18</v>
       </c>
       <c r="C121" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="inlineStr"/>
@@ -2999,7 +2999,7 @@
         <v>18</v>
       </c>
       <c r="C122" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr"/>
@@ -3038,7 +3038,7 @@
         <v>19</v>
       </c>
       <c r="C125" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D125" t="inlineStr"/>
       <c r="E125" t="inlineStr"/>
@@ -3155,7 +3155,7 @@
         <v>25</v>
       </c>
       <c r="C134" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D134" t="inlineStr"/>
       <c r="E134" t="inlineStr"/>
@@ -3207,7 +3207,7 @@
         <v>25</v>
       </c>
       <c r="C138" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D138" t="inlineStr"/>
       <c r="E138" t="inlineStr"/>
@@ -3220,7 +3220,7 @@
         <v>27</v>
       </c>
       <c r="C139" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D139" t="inlineStr"/>
       <c r="E139" t="inlineStr"/>
@@ -3246,7 +3246,7 @@
         <v>27</v>
       </c>
       <c r="C141" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D141" t="inlineStr"/>
       <c r="E141" t="inlineStr"/>
@@ -3272,7 +3272,7 @@
         <v>29</v>
       </c>
       <c r="C143" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D143" t="inlineStr"/>
       <c r="E143" t="inlineStr"/>
@@ -3337,7 +3337,7 @@
         <v>30</v>
       </c>
       <c r="C148" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="D148" t="inlineStr"/>
       <c r="E148" t="inlineStr"/>
@@ -3350,7 +3350,7 @@
         <v>30</v>
       </c>
       <c r="C149" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D149" t="inlineStr"/>
       <c r="E149" t="inlineStr"/>
@@ -3454,7 +3454,7 @@
         <v>36</v>
       </c>
       <c r="C157" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D157" t="inlineStr"/>
       <c r="E157" t="inlineStr"/>
@@ -3467,7 +3467,7 @@
         <v>36</v>
       </c>
       <c r="C158" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D158" t="inlineStr"/>
       <c r="E158" t="inlineStr"/>

</xml_diff>

<commit_message>
Removed MTZ, fixed linearization, changed data
</commit_message>
<xml_diff>
--- a/data/37-intersection map EV1 Solution.xlsx
+++ b/data/37-intersection map EV1 Solution.xlsx
@@ -489,16 +489,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>16.1754615237336</v>
+        <v>11.37314754853339</v>
       </c>
       <c r="D2" t="n">
-        <v>16.1754615237336</v>
+        <v>11.37314754853339</v>
       </c>
       <c r="E2" t="n">
-        <v>9.364289244444443</v>
+        <v>9.161042399999994</v>
       </c>
       <c r="F2" t="n">
-        <v>9.364289244444443</v>
+        <v>9.161042399999994</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -512,16 +512,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>14.53785325040029</v>
+        <v>9.735539275200056</v>
       </c>
       <c r="D3" t="n">
-        <v>14.53785325040029</v>
+        <v>9.735539275200056</v>
       </c>
       <c r="E3" t="n">
-        <v>9.732904799999998</v>
+        <v>9.52965795555555</v>
       </c>
       <c r="F3" t="n">
-        <v>9.982904799999998</v>
+        <v>9.77965795555555</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -534,7 +534,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -557,7 +557,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -580,7 +580,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -603,7 +603,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -629,16 +629,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>14.35195164373362</v>
+        <v>9.549637668533389</v>
       </c>
       <c r="D8" t="n">
-        <v>14.35195164373362</v>
+        <v>9.549637668533389</v>
       </c>
       <c r="E8" t="n">
-        <v>10.02485368888889</v>
+        <v>9.821606844444439</v>
       </c>
       <c r="F8" t="n">
-        <v>10.02485368888889</v>
+        <v>9.821606844444439</v>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
@@ -652,16 +652,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>12.93654337040032</v>
+        <v>8.134229395200055</v>
       </c>
       <c r="D9" t="n">
-        <v>12.93654337040032</v>
+        <v>8.134229395200055</v>
       </c>
       <c r="E9" t="n">
-        <v>10.34346924444444</v>
+        <v>10.1402224</v>
       </c>
       <c r="F9" t="n">
-        <v>10.34346924444444</v>
+        <v>10.1402224</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
@@ -675,16 +675,16 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>10.70640176373369</v>
+        <v>5.904087788533426</v>
       </c>
       <c r="D10" t="n">
-        <v>10.70640176373369</v>
+        <v>5.904087788533426</v>
       </c>
       <c r="E10" t="n">
-        <v>10.84541813333333</v>
+        <v>10.64217128888888</v>
       </c>
       <c r="F10" t="n">
-        <v>11.09541813333333</v>
+        <v>10.89217128888888</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
@@ -700,16 +700,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>17.6589475485336</v>
+        <v>12.85663357333337</v>
       </c>
       <c r="D11" t="n">
-        <v>17.6589475485336</v>
+        <v>12.85663357333337</v>
       </c>
       <c r="E11" t="n">
-        <v>9.161042399999998</v>
+        <v>8.957795555555549</v>
       </c>
       <c r="F11" t="n">
-        <v>9.161042399999998</v>
+        <v>8.957795555555549</v>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
@@ -720,22 +720,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>18.41223357333357</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>18.41223357333357</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>9.057795555555554</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>9.057795555555554</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -747,7 +747,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -770,7 +770,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -793,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -808,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -823,22 +823,22 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>10.17979349040035</v>
+        <v>5.377479515200092</v>
       </c>
       <c r="D16" t="n">
-        <v>22.8969416066667</v>
+        <v>11.2408268181331</v>
       </c>
       <c r="E16" t="n">
-        <v>11.21403368888889</v>
+        <v>11.01078684444444</v>
       </c>
       <c r="F16" t="n">
-        <v>14.89376404660485</v>
+        <v>12.70735724459867</v>
       </c>
       <c r="G16" t="n">
         <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>3.679730357715957</v>
+        <v>1.696570400154228</v>
       </c>
       <c r="I16" t="inlineStr"/>
     </row>
@@ -850,16 +850,16 @@
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>22</v>
+        <v>10.34388521146644</v>
       </c>
       <c r="D17" t="n">
-        <v>22</v>
+        <v>10.34388521146644</v>
       </c>
       <c r="E17" t="n">
-        <v>15.09571293549373</v>
+        <v>12.90930613348756</v>
       </c>
       <c r="F17" t="n">
-        <v>15.09571293549373</v>
+        <v>12.90930613348756</v>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
@@ -873,16 +873,16 @@
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>21.47339172666676</v>
+        <v>9.817276938133105</v>
       </c>
       <c r="D18" t="n">
-        <v>21.47339172666676</v>
+        <v>9.817276938133105</v>
       </c>
       <c r="E18" t="n">
-        <v>15.21432849104929</v>
+        <v>13.02792168904311</v>
       </c>
       <c r="F18" t="n">
-        <v>15.21432849104929</v>
+        <v>13.02792168904311</v>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
@@ -919,16 +919,16 @@
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>19.3832418466669</v>
+        <v>13.3832418466667</v>
       </c>
       <c r="D20" t="n">
-        <v>19.3832418466669</v>
+        <v>13.3832418466667</v>
       </c>
       <c r="E20" t="n">
-        <v>8.589179999999999</v>
+        <v>8.589180000000011</v>
       </c>
       <c r="F20" t="n">
-        <v>8.839179999999999</v>
+        <v>8.839180000000011</v>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -967,16 +967,16 @@
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>20.28018345333334</v>
+        <v>14.28018345333336</v>
       </c>
       <c r="D22" t="n">
-        <v>20.28018345333334</v>
+        <v>14.28018345333336</v>
       </c>
       <c r="E22" t="n">
-        <v>8.387231111111111</v>
+        <v>8.387231111111122</v>
       </c>
       <c r="F22" t="n">
-        <v>8.387231111111111</v>
+        <v>8.387231111111122</v>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
@@ -1013,16 +1013,16 @@
         <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>20.95492506000001</v>
+        <v>14.95492506</v>
       </c>
       <c r="D24" t="n">
-        <v>20.95492506000001</v>
+        <v>14.95492506</v>
       </c>
       <c r="E24" t="n">
-        <v>8.235282222222223</v>
+        <v>8.235282222222231</v>
       </c>
       <c r="F24" t="n">
-        <v>8.235282222222223</v>
+        <v>8.235282222222231</v>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
@@ -1036,10 +1036,10 @@
         <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D25" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E25" t="n">
         <v>8</v>
@@ -1059,16 +1059,16 @@
         <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>16.1964542152001</v>
+        <v>16.74880827333331</v>
       </c>
       <c r="D26" t="n">
-        <v>16.1964542152001</v>
+        <v>16.74880827333331</v>
       </c>
       <c r="E26" t="n">
-        <v>16.47008866882707</v>
+        <v>18.33692864459871</v>
       </c>
       <c r="F26" t="n">
-        <v>16.72008866882707</v>
+        <v>18.58692864459871</v>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
@@ -1081,25 +1081,25 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>14.71296819040009</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>23.63760827333332</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>16.92333551327151</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>18.33189613242133</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>1.408560619149816</v>
+        <v>0</v>
       </c>
       <c r="I27" t="inlineStr"/>
     </row>
@@ -1108,19 +1108,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>18.26410024000009</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>18.26410024000009</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>16.18684182438262</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>16.18684182438262</v>
+        <v>0</v>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
@@ -1154,19 +1154,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>19.67950851333343</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>19.67950851333343</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>15.86822626882707</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>15.86822626882707</v>
+        <v>0</v>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
@@ -1180,16 +1180,16 @@
         <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>20.20611678666676</v>
+        <v>8.550001998133123</v>
       </c>
       <c r="D31" t="n">
-        <v>20.20611678666676</v>
+        <v>8.550001998133123</v>
       </c>
       <c r="E31" t="n">
-        <v>15.49961071327151</v>
+        <v>13.31320391126533</v>
       </c>
       <c r="F31" t="n">
-        <v>15.74961071327151</v>
+        <v>13.56320391126533</v>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
@@ -1202,7 +1202,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -1271,7 +1271,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -1294,7 +1294,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -1317,19 +1317,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>7.28272705813311</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>7.28272705813311</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>13.84848613348755</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>13.84848613348755</v>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
@@ -1340,25 +1340,25 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>5.722654298133106</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>19.54665429813329</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>13.95368180015422</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>17.95368180015427</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I38" t="inlineStr"/>
     </row>
@@ -1370,16 +1370,16 @@
         <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D39" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E39" t="n">
-        <v>18.70051168797688</v>
+        <v>18.75554420015427</v>
       </c>
       <c r="F39" t="n">
-        <v>18.70051168797688</v>
+        <v>18.75554420015427</v>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
@@ -1396,7 +1396,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1439,7 +1439,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -1452,7 +1452,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -1504,7 +1504,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
@@ -1517,7 +1517,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
@@ -1543,7 +1543,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -1556,7 +1556,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -1569,7 +1569,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -1582,7 +1582,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
@@ -1595,7 +1595,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
@@ -1608,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
@@ -1634,7 +1634,7 @@
         <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
@@ -1660,7 +1660,7 @@
         <v>15</v>
       </c>
       <c r="C19" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
@@ -1686,7 +1686,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
@@ -1696,7 +1696,7 @@
         <v>10</v>
       </c>
       <c r="B22" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -1706,10 +1706,10 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
+        <v>10</v>
+      </c>
+      <c r="B23" t="n">
         <v>11</v>
-      </c>
-      <c r="B23" t="n">
-        <v>19</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -1722,7 +1722,7 @@
         <v>11</v>
       </c>
       <c r="B24" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -1732,13 +1732,13 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C25" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
@@ -1748,36 +1748,36 @@
         <v>12</v>
       </c>
       <c r="B26" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C26" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C27" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B28" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
@@ -1787,10 +1787,10 @@
         <v>14</v>
       </c>
       <c r="B29" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C29" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
@@ -1800,36 +1800,36 @@
         <v>14</v>
       </c>
       <c r="B30" t="n">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C30" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" t="n">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
+        <v>15</v>
+      </c>
+      <c r="B32" t="n">
         <v>16</v>
       </c>
-      <c r="B32" t="n">
-        <v>8</v>
-      </c>
       <c r="C32" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
@@ -1839,10 +1839,10 @@
         <v>16</v>
       </c>
       <c r="B33" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
@@ -1852,10 +1852,10 @@
         <v>16</v>
       </c>
       <c r="B34" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
@@ -1865,23 +1865,23 @@
         <v>16</v>
       </c>
       <c r="B35" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C36" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
@@ -1891,20 +1891,20 @@
         <v>17</v>
       </c>
       <c r="B37" t="n">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C37" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -1917,10 +1917,10 @@
         <v>18</v>
       </c>
       <c r="B39" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
@@ -1930,7 +1930,7 @@
         <v>18</v>
       </c>
       <c r="B40" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -1956,7 +1956,7 @@
         <v>19</v>
       </c>
       <c r="B42" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -1969,7 +1969,7 @@
         <v>19</v>
       </c>
       <c r="B43" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -1979,10 +1979,10 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B44" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -1992,10 +1992,10 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
+        <v>20</v>
+      </c>
+      <c r="B45" t="n">
         <v>21</v>
-      </c>
-      <c r="B45" t="n">
-        <v>28</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -2005,26 +2005,26 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B46" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C46" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B47" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
@@ -2034,20 +2034,20 @@
         <v>23</v>
       </c>
       <c r="B48" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
+        <v>23</v>
+      </c>
+      <c r="B49" t="n">
         <v>24</v>
-      </c>
-      <c r="B49" t="n">
-        <v>20</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -2060,7 +2060,7 @@
         <v>24</v>
       </c>
       <c r="B50" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -2073,20 +2073,20 @@
         <v>24</v>
       </c>
       <c r="B51" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C51" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B52" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -2099,10 +2099,10 @@
         <v>25</v>
       </c>
       <c r="B53" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
@@ -2112,7 +2112,7 @@
         <v>25</v>
       </c>
       <c r="B54" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
@@ -2125,10 +2125,10 @@
         <v>25</v>
       </c>
       <c r="B55" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C55" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
@@ -2138,7 +2138,7 @@
         <v>25</v>
       </c>
       <c r="B56" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B57" t="n">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C57" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr"/>
@@ -2164,10 +2164,10 @@
         <v>27</v>
       </c>
       <c r="B58" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C58" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
@@ -2177,10 +2177,10 @@
         <v>27</v>
       </c>
       <c r="B59" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C59" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr"/>
@@ -2190,23 +2190,23 @@
         <v>27</v>
       </c>
       <c r="B60" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C60" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B61" t="n">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C61" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
@@ -2216,10 +2216,10 @@
         <v>29</v>
       </c>
       <c r="B62" t="n">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
@@ -2229,7 +2229,7 @@
         <v>29</v>
       </c>
       <c r="B63" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
@@ -2242,23 +2242,23 @@
         <v>29</v>
       </c>
       <c r="B64" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C64" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B65" t="n">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C65" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr"/>
@@ -2268,10 +2268,10 @@
         <v>30</v>
       </c>
       <c r="B66" t="n">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C66" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
@@ -2281,7 +2281,7 @@
         <v>30</v>
       </c>
       <c r="B67" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
@@ -2291,39 +2291,39 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B68" t="n">
         <v>36</v>
       </c>
       <c r="C68" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B69" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C69" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B70" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C70" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
@@ -2333,23 +2333,23 @@
         <v>33</v>
       </c>
       <c r="B71" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C71" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B72" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C72" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
@@ -2359,36 +2359,36 @@
         <v>34</v>
       </c>
       <c r="B73" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C73" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
+        <v>34</v>
+      </c>
+      <c r="B74" t="n">
         <v>35</v>
       </c>
-      <c r="B74" t="n">
-        <v>36</v>
-      </c>
       <c r="C74" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
+        <v>35</v>
+      </c>
+      <c r="B75" t="n">
         <v>36</v>
       </c>
-      <c r="B75" t="n">
-        <v>32</v>
-      </c>
       <c r="C75" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr"/>
@@ -2398,7 +2398,7 @@
         <v>36</v>
       </c>
       <c r="B76" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C76" t="n">
         <v>0</v>
@@ -2408,13 +2408,13 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
+        <v>36</v>
+      </c>
+      <c r="B77" t="n">
         <v>37</v>
       </c>
-      <c r="B77" t="n">
-        <v>34</v>
-      </c>
       <c r="C77" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr"/>
@@ -2424,20 +2424,20 @@
         <v>37</v>
       </c>
       <c r="B78" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C78" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B79" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C79" t="n">
         <v>0</v>
@@ -2450,7 +2450,7 @@
         <v>38</v>
       </c>
       <c r="B80" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C80" t="n">
         <v>0</v>
@@ -2463,7 +2463,7 @@
         <v>38</v>
       </c>
       <c r="B81" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C81" t="n">
         <v>0</v>
@@ -2473,10 +2473,10 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B82" t="n">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C82" t="n">
         <v>0</v>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B83" t="n">
         <v>38</v>
@@ -2499,36 +2499,36 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B84" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B85" t="n">
         <v>1</v>
       </c>
       <c r="C85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C86" t="n">
         <v>1</v>
@@ -2538,36 +2538,36 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B87" t="n">
         <v>2</v>
       </c>
       <c r="C87" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B88" t="n">
         <v>2</v>
       </c>
       <c r="C88" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
+        <v>7</v>
+      </c>
+      <c r="B89" t="n">
         <v>2</v>
-      </c>
-      <c r="B89" t="n">
-        <v>3</v>
       </c>
       <c r="C89" t="n">
         <v>0</v>
@@ -2577,20 +2577,20 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
+        <v>2</v>
+      </c>
+      <c r="B90" t="n">
         <v>3</v>
       </c>
-      <c r="B90" t="n">
-        <v>4</v>
-      </c>
       <c r="C90" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B91" t="n">
         <v>4</v>
@@ -2603,130 +2603,130 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B92" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C92" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B93" t="n">
         <v>5</v>
       </c>
       <c r="C93" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B94" t="n">
         <v>5</v>
       </c>
       <c r="C94" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C95" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B96" t="n">
         <v>6</v>
       </c>
       <c r="C96" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B97" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C97" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B98" t="n">
         <v>7</v>
       </c>
       <c r="C98" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B99" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C99" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B100" t="n">
         <v>8</v>
       </c>
       <c r="C100" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B101" t="n">
         <v>8</v>
       </c>
       <c r="C101" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr"/>
@@ -2736,17 +2736,17 @@
         <v>15</v>
       </c>
       <c r="B102" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C102" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B103" t="n">
         <v>9</v>
@@ -2759,13 +2759,13 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B104" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C104" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr"/>
@@ -2775,7 +2775,7 @@
         <v>19</v>
       </c>
       <c r="B105" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C105" t="n">
         <v>1</v>
@@ -2785,10 +2785,10 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B106" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C106" t="n">
         <v>0</v>
@@ -2798,78 +2798,78 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B107" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C107" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B108" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C108" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B109" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C109" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B110" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C110" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B111" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C111" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B112" t="n">
         <v>14</v>
       </c>
       <c r="C112" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
@@ -2879,56 +2879,56 @@
         <v>16</v>
       </c>
       <c r="B113" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C113" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B114" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C114" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B115" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C115" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B116" t="n">
         <v>16</v>
       </c>
       <c r="C116" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B117" t="n">
         <v>16</v>
@@ -2944,46 +2944,46 @@
         <v>18</v>
       </c>
       <c r="B118" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C118" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B119" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C119" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B120" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C120" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B121" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C121" t="n">
         <v>0</v>
@@ -2993,7 +2993,7 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B122" t="n">
         <v>18</v>
@@ -3006,10 +3006,10 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B123" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C123" t="n">
         <v>0</v>
@@ -3019,20 +3019,20 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B124" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B125" t="n">
         <v>19</v>
@@ -3048,10 +3048,10 @@
         <v>21</v>
       </c>
       <c r="B126" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C126" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="D126" t="inlineStr"/>
       <c r="E126" t="inlineStr"/>
@@ -3061,20 +3061,20 @@
         <v>28</v>
       </c>
       <c r="B127" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C127" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B128" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C128" t="n">
         <v>0</v>
@@ -3084,36 +3084,36 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
+        <v>28</v>
+      </c>
+      <c r="B129" t="n">
         <v>21</v>
       </c>
-      <c r="B129" t="n">
-        <v>23</v>
-      </c>
       <c r="C129" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B130" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C130" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B131" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C131" t="n">
         <v>0</v>
@@ -3123,20 +3123,20 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B132" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B133" t="n">
         <v>24</v>
@@ -3149,10 +3149,10 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
+        <v>22</v>
+      </c>
+      <c r="B134" t="n">
         <v>24</v>
-      </c>
-      <c r="B134" t="n">
-        <v>25</v>
       </c>
       <c r="C134" t="n">
         <v>0</v>
@@ -3165,7 +3165,7 @@
         <v>26</v>
       </c>
       <c r="B135" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C135" t="n">
         <v>0</v>
@@ -3175,33 +3175,33 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B136" t="n">
         <v>25</v>
       </c>
       <c r="C136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D136" t="inlineStr"/>
       <c r="E136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B137" t="n">
         <v>25</v>
       </c>
       <c r="C137" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D137" t="inlineStr"/>
       <c r="E137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B138" t="n">
         <v>25</v>
@@ -3214,10 +3214,10 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B139" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C139" t="n">
         <v>0</v>
@@ -3227,20 +3227,20 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B140" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C140" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="D140" t="inlineStr"/>
       <c r="E140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B141" t="n">
         <v>27</v>
@@ -3253,23 +3253,23 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B142" t="n">
         <v>27</v>
       </c>
       <c r="C142" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D142" t="inlineStr"/>
       <c r="E142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B143" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C143" t="n">
         <v>0</v>
@@ -3279,143 +3279,143 @@
     </row>
     <row r="144">
       <c r="A144" t="n">
+        <v>35</v>
+      </c>
+      <c r="B144" t="n">
         <v>27</v>
       </c>
-      <c r="B144" t="n">
-        <v>29</v>
-      </c>
       <c r="C144" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D144" t="inlineStr"/>
       <c r="E144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B145" t="n">
         <v>29</v>
       </c>
       <c r="C145" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D145" t="inlineStr"/>
       <c r="E145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B146" t="n">
         <v>29</v>
       </c>
       <c r="C146" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D146" t="inlineStr"/>
       <c r="E146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B147" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D147" t="inlineStr"/>
       <c r="E147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B148" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C148" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D148" t="inlineStr"/>
       <c r="E148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B149" t="n">
         <v>30</v>
       </c>
       <c r="C149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D149" t="inlineStr"/>
       <c r="E149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B150" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C150" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D150" t="inlineStr"/>
       <c r="E150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B151" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C151" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D151" t="inlineStr"/>
       <c r="E151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B152" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C152" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D152" t="inlineStr"/>
       <c r="E152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B153" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C153" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D153" t="inlineStr"/>
       <c r="E153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B154" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C154" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D154" t="inlineStr"/>
       <c r="E154" t="inlineStr"/>
@@ -3425,33 +3425,33 @@
         <v>35</v>
       </c>
       <c r="B155" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C155" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D155" t="inlineStr"/>
       <c r="E155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B156" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C156" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D156" t="inlineStr"/>
       <c r="E156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B157" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C157" t="n">
         <v>0</v>
@@ -3461,10 +3461,10 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B158" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C158" t="n">
         <v>0</v>
@@ -3474,36 +3474,36 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B159" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C159" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D159" t="inlineStr"/>
       <c r="E159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B160" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C160" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D160" t="inlineStr"/>
       <c r="E160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B161" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C161" t="n">
         <v>0</v>
@@ -3513,10 +3513,10 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B162" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C162" t="n">
         <v>0</v>
@@ -3526,23 +3526,23 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B163" t="n">
         <v>38</v>
       </c>
       <c r="C163" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D163" t="inlineStr"/>
       <c r="E163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="n">
+        <v>22</v>
+      </c>
+      <c r="B164" t="n">
         <v>38</v>
-      </c>
-      <c r="B164" t="n">
-        <v>23</v>
       </c>
       <c r="C164" t="n">
         <v>0</v>
@@ -3552,16 +3552,42 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
+        <v>26</v>
+      </c>
+      <c r="B165" t="n">
         <v>38</v>
-      </c>
-      <c r="B165" t="n">
-        <v>25</v>
       </c>
       <c r="C165" t="n">
         <v>0</v>
       </c>
       <c r="D165" t="inlineStr"/>
       <c r="E165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>38</v>
+      </c>
+      <c r="B166" t="n">
+        <v>23</v>
+      </c>
+      <c r="C166" t="n">
+        <v>0</v>
+      </c>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr"/>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>38</v>
+      </c>
+      <c r="B167" t="n">
+        <v>25</v>
+      </c>
+      <c r="C167" t="n">
+        <v>0</v>
+      </c>
+      <c r="D167" t="inlineStr"/>
+      <c r="E167" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>